<commit_message>
Weekly Project Update Log by Snehal
</commit_message>
<xml_diff>
--- a/docs/ProjectLog.xlsx
+++ b/docs/ProjectLog.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snehi23/Desktop/SF/code/Pivi_-_Plugin_For_Visual_Parallel_Programming/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team Weekly Tasks" sheetId="1" r:id="rId1"/>
@@ -17,9 +22,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Team Weekly Tasks'!$A$1:$E$7</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>Start Date</t>
   </si>
@@ -175,11 +186,68 @@
 4. Completed writing about Architectural Strategies team can make use of for this project.
 5. Still need to work on architecture of the project.</t>
   </si>
+  <si>
+    <t>1. Reviewed the project proposal.
+2. Had a meeting with sponsor about understanding prpject in details
+3. Participated in meeting with team and discussed about project goals</t>
+  </si>
+  <si>
+    <t>Got some basic understanding of project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Brainstormed about the requirements with the team and listed the questions for sponsors
+2. Met the sponsor to clarify on those questions
+3. Worked on section 1 &amp; 3  of Project charter
+</t>
+  </si>
+  <si>
+    <t>1. Got clarification on the questions asked to sponsors 
+2. Completed section 1 &amp; 3 in Project Charter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Researched on possible libraries and software required for the project       2. Set up git account, taiga scrum board and slack communication channel and intercommunication between tools. </t>
+  </si>
+  <si>
+    <t>1. Found that GMF is supposably to be used for this project                                                              2. All accounts and software setup is done.</t>
+  </si>
+  <si>
+    <t>1. Made update on sections of project charter as per sponsor's comments.
+2. Brainstormed on Functional requirements of the project.
+3. Worked on External Interface requirements, Functional requirements, Software Quality Attributes in SRS.
+4. Tried plugin development on local to understand the technology.
+6. Researched on GMF and corresponding libraries require for project.</t>
+  </si>
+  <si>
+    <t>1. Completed changes to project charter.
+2. Completed documention External Interface Requirement, Software Quality Attribute sections in SRS.
+3. Shared undestanding with team about plugin development.
+4. Found that GMF combines both EMF and GEF and can be used for the project.</t>
+  </si>
+  <si>
+    <t>1. Made changes to External Interface Requirements, Functional Requirements in SRS based on the sponsors comments.
+2. Reseached on EMF Ecore models.
+3. Started  working on design of project and worked on the section 1 &amp; 2 of SDS.</t>
+  </si>
+  <si>
+    <t>1. Completed changes to SRS
+2. Figured out EMF Ecore model necessity.
+3. Completed the first two sections of SDS.
+4. Working on detailed design of project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>1. Worked on Use Cases for each core functionalities of project                        2. Worked on Policies and Tacticis of SDS                                                              3. Shared EMF demo code with team mates and explain my understanding</t>
+  </si>
+  <si>
+    <t>1. Use Case is integrated in SRS and some minor comments by spnosor.                                2. Completed Policies and Tactics part of SDS      3. Working on detailed design of project             4.  EMF demo is shared on git for all team members</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -549,19 +617,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="82.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -578,7 +646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -595,7 +663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -612,7 +680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -629,7 +697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="135" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -646,7 +714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="150" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -663,7 +731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -689,18 +757,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.28515625" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.33203125" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -717,7 +785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -734,7 +802,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -751,7 +819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -768,7 +836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -785,7 +853,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -802,7 +870,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -827,13 +895,13 @@
       <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.28515625" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -850,7 +918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -861,7 +929,7 @@
         <v>42669</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -872,7 +940,7 @@
         <v>42676</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -883,7 +951,7 @@
         <v>42683</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -894,7 +962,7 @@
         <v>42690</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -905,7 +973,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -925,17 +993,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -952,7 +1023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -962,8 +1033,14 @@
       <c r="C2" s="2">
         <v>42669</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -973,8 +1050,14 @@
       <c r="C3" s="2">
         <v>42676</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -984,8 +1067,14 @@
       <c r="C4" s="2">
         <v>42683</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -995,8 +1084,14 @@
       <c r="C5" s="2">
         <v>42690</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1006,16 +1101,28 @@
       <c r="C6" s="2">
         <v>42697</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>42698</v>
       </c>
-      <c r="C7" s="2">
-        <v>42673</v>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1031,13 +1138,13 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.42578125" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1054,7 +1161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1065,7 +1172,7 @@
         <v>42669</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1076,7 +1183,7 @@
         <v>42676</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1087,7 +1194,7 @@
         <v>42683</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1098,7 +1205,7 @@
         <v>42690</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1109,7 +1216,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1133,13 +1240,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.5703125" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1156,7 +1263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1167,7 +1274,7 @@
         <v>42669</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1178,7 +1285,7 @@
         <v>42676</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1189,7 +1296,7 @@
         <v>42683</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1200,7 +1307,7 @@
         <v>42690</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1211,7 +1318,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>